<commit_message>
feat: update week 4
</commit_message>
<xml_diff>
--- a/Data_Engineering_Training .xlsx
+++ b/Data_Engineering_Training .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kyanon\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77F5D2B-2E53-4B37-854B-75EB0FC2DC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF9CF97-03DB-4150-816C-E44230DFE65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="75">
   <si>
     <t>Week</t>
   </si>
@@ -726,6 +726,18 @@
   <si>
     <t>- Spark</t>
   </si>
+  <si>
+    <t>13/12/2025</t>
+  </si>
+  <si>
+    <t>- Completed Feature Engineering task</t>
+  </si>
+  <si>
+    <t>14/12/2025</t>
+  </si>
+  <si>
+    <t>16/12/2025</t>
+  </si>
 </sst>
 </file>
 
@@ -1075,20 +1087,20 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1307,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1053"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E21" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="F22" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1350,12 +1362,12 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="43.2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1474,12 +1486,12 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="28.8">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="43"/>
       <c r="E9" s="3" t="s">
         <v>31</v>
       </c>
@@ -1594,12 +1606,12 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="28.8">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="43"/>
       <c r="E16" s="3" t="s">
         <v>36</v>
       </c>
@@ -1696,12 +1708,12 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="42"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="43"/>
       <c r="E22" s="20" t="s">
         <v>41</v>
       </c>
@@ -1716,7 +1728,7 @@
       <c r="B23" s="18"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="48" t="s">
+      <c r="E23" s="40" t="s">
         <v>43</v>
       </c>
       <c r="F23" s="9"/>
@@ -1741,43 +1753,63 @@
       <c r="G24" s="9"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="1:8" ht="29.4" customHeight="1">
+    <row r="25" spans="1:8" ht="39" customHeight="1">
       <c r="A25" s="5"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="6"/>
+      <c r="B25" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>12</v>
+      </c>
       <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="E25" s="39" t="s">
+        <v>68</v>
+      </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="6"/>
+      <c r="H25" s="34" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="26" spans="1:8" ht="39" customHeight="1">
       <c r="A26" s="5"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="6"/>
+      <c r="B26" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>12</v>
+      </c>
       <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="E26" s="39" t="s">
+        <v>70</v>
+      </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8" ht="64.8" customHeight="1">
       <c r="A27" s="5"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="6"/>
+      <c r="B27" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>12</v>
+      </c>
       <c r="D27" s="6"/>
-      <c r="E27" s="19"/>
+      <c r="E27" s="39" t="s">
+        <v>70</v>
+      </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="6"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A28" s="40" t="s">
+      <c r="A28" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="42"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="43"/>
       <c r="E28" s="20" t="s">
         <v>46</v>
       </c>
@@ -1866,12 +1898,12 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="42"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="43"/>
       <c r="E36" s="20"/>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
@@ -12049,6 +12081,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A28:D28"/>
     <mergeCell ref="A36:D36"/>
     <mergeCell ref="A297:A298"/>
     <mergeCell ref="A299:A300"/>
@@ -12060,11 +12097,6 @@
     <mergeCell ref="B266:B267"/>
     <mergeCell ref="B297:B298"/>
     <mergeCell ref="B299:B300"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A28:D28"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="C3:C8 C10:C15 C42:C1047 C23:C27 C29:C35 C17:C21" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>

<commit_message>
feat: update week 5
</commit_message>
<xml_diff>
--- a/Data_Engineering_Training .xlsx
+++ b/Data_Engineering_Training .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kyanon\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB50BD26-A3B9-4A5B-8B22-814DD02B159E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2311FCF4-F6D2-4298-8EAA-4A7E084CB995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="90">
   <si>
     <t>Week</t>
   </si>
@@ -751,10 +751,37 @@
     <t>19/12/2025</t>
   </si>
   <si>
-    <t>22/12/2025</t>
+    <t>- Completed Detailed Table &amp; Filters task</t>
   </si>
   <si>
-    <t>- Completed Detailed Table &amp; Filters task</t>
+    <t>23/12/2025</t>
+  </si>
+  <si>
+    <t>- Cloud components</t>
+  </si>
+  <si>
+    <t>24/12/2025</t>
+  </si>
+  <si>
+    <t>- Research cloud components used in data engineer</t>
+  </si>
+  <si>
+    <t>25/12/2025</t>
+  </si>
+  <si>
+    <t>- Cloud etl pipeline</t>
+  </si>
+  <si>
+    <t>- Completed 3 task: cloud compute logic, file renaming &amp; moving, data warehouse load</t>
+  </si>
+  <si>
+    <t>26/12/2025</t>
+  </si>
+  <si>
+    <t>- Cloud components, BI tools</t>
+  </si>
+  <si>
+    <t>- Review Cloud components used in data, comparison BI tools</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1033,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1108,18 +1135,21 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1337,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1053"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F24" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1380,7 +1410,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="43.2">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="48" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="42"/>
@@ -1504,7 +1534,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="28.8">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="48" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="42"/>
@@ -1624,7 +1654,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="28.8">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="48" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="42"/>
@@ -1726,7 +1756,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="48" t="s">
         <v>40</v>
       </c>
       <c r="B22" s="42"/>
@@ -1828,7 +1858,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A28" s="41" t="s">
+      <c r="A28" s="48" t="s">
         <v>45</v>
       </c>
       <c r="B28" s="42"/>
@@ -1841,14 +1871,14 @@
       <c r="G28" s="14"/>
       <c r="H28" s="15"/>
     </row>
-    <row r="29" spans="1:8" ht="135.6" customHeight="1">
+    <row r="29" spans="1:8" ht="160.19999999999999" customHeight="1">
       <c r="A29" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="18"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="7" t="s">
         <v>48</v>
       </c>
       <c r="F29" s="9"/>
@@ -1860,7 +1890,7 @@
     <row r="30" spans="1:8" ht="40.200000000000003" customHeight="1">
       <c r="A30" s="5"/>
       <c r="B30" s="38" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C30" s="35" t="s">
         <v>12</v>
@@ -1872,40 +1902,64 @@
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="34.799999999999997" customHeight="1">
       <c r="A31" s="5"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="6"/>
+      <c r="B31" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>12</v>
+      </c>
       <c r="D31" s="6"/>
-      <c r="E31" s="16"/>
+      <c r="E31" s="39" t="s">
+        <v>81</v>
+      </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
-      <c r="H31" s="6"/>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1">
+      <c r="H31" s="34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="39" customHeight="1">
       <c r="A32" s="5"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="6"/>
+      <c r="B32" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>12</v>
+      </c>
       <c r="D32" s="6"/>
-      <c r="E32" s="16"/>
+      <c r="E32" s="39" t="s">
+        <v>85</v>
+      </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
-      <c r="H32" s="6"/>
-    </row>
-    <row r="33" spans="1:8" ht="15.75" customHeight="1">
+      <c r="H32" s="34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="47.4" customHeight="1">
       <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
+      <c r="B33" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>12</v>
+      </c>
       <c r="D33" s="6"/>
-      <c r="E33" s="16"/>
+      <c r="E33" s="39" t="s">
+        <v>88</v>
+      </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
-      <c r="H33" s="6"/>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" customHeight="1">
+      <c r="H33" s="34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="37.799999999999997" customHeight="1">
       <c r="A34" s="5"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -1930,7 +1984,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="41" t="s">
         <v>52</v>
       </c>
       <c r="B36" s="42"/>
@@ -3062,8 +3116,8 @@
       <c r="H148" s="6"/>
     </row>
     <row r="149" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A149" s="47"/>
-      <c r="B149" s="47"/>
+      <c r="A149" s="46"/>
+      <c r="B149" s="46"/>
       <c r="C149" s="6"/>
       <c r="D149" s="6"/>
       <c r="E149" s="6"/>
@@ -3072,8 +3126,8 @@
       <c r="H149" s="6"/>
     </row>
     <row r="150" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A150" s="46"/>
-      <c r="B150" s="46"/>
+      <c r="A150" s="45"/>
+      <c r="B150" s="45"/>
       <c r="C150" s="6"/>
       <c r="D150" s="6"/>
       <c r="E150" s="6"/>
@@ -3082,8 +3136,8 @@
       <c r="H150" s="6"/>
     </row>
     <row r="151" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A151" s="48"/>
-      <c r="B151" s="48"/>
+      <c r="A151" s="47"/>
+      <c r="B151" s="47"/>
       <c r="C151" s="6"/>
       <c r="D151" s="6"/>
       <c r="E151" s="6"/>
@@ -3092,8 +3146,8 @@
       <c r="H151" s="6"/>
     </row>
     <row r="152" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A152" s="46"/>
-      <c r="B152" s="46"/>
+      <c r="A152" s="45"/>
+      <c r="B152" s="45"/>
       <c r="C152" s="6"/>
       <c r="D152" s="6"/>
       <c r="E152" s="6"/>
@@ -4232,8 +4286,8 @@
       <c r="H265" s="6"/>
     </row>
     <row r="266" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A266" s="47"/>
-      <c r="B266" s="47"/>
+      <c r="A266" s="46"/>
+      <c r="B266" s="46"/>
       <c r="C266" s="6"/>
       <c r="D266" s="6"/>
       <c r="E266" s="6"/>
@@ -4242,8 +4296,8 @@
       <c r="H266" s="6"/>
     </row>
     <row r="267" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A267" s="46"/>
-      <c r="B267" s="46"/>
+      <c r="A267" s="45"/>
+      <c r="B267" s="45"/>
       <c r="C267" s="6"/>
       <c r="D267" s="6"/>
       <c r="E267" s="6"/>
@@ -4542,8 +4596,8 @@
       <c r="H296" s="6"/>
     </row>
     <row r="297" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A297" s="45"/>
-      <c r="B297" s="45"/>
+      <c r="A297" s="44"/>
+      <c r="B297" s="44"/>
       <c r="C297" s="6"/>
       <c r="D297" s="6"/>
       <c r="E297" s="6"/>
@@ -4552,8 +4606,8 @@
       <c r="H297" s="6"/>
     </row>
     <row r="298" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A298" s="46"/>
-      <c r="B298" s="46"/>
+      <c r="A298" s="45"/>
+      <c r="B298" s="45"/>
       <c r="C298" s="6"/>
       <c r="D298" s="6"/>
       <c r="E298" s="6"/>
@@ -4562,8 +4616,8 @@
       <c r="H298" s="6"/>
     </row>
     <row r="299" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A299" s="47"/>
-      <c r="B299" s="47"/>
+      <c r="A299" s="46"/>
+      <c r="B299" s="46"/>
       <c r="C299" s="6"/>
       <c r="D299" s="6"/>
       <c r="E299" s="6"/>
@@ -4572,8 +4626,8 @@
       <c r="H299" s="28"/>
     </row>
     <row r="300" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A300" s="46"/>
-      <c r="B300" s="46"/>
+      <c r="A300" s="45"/>
+      <c r="B300" s="45"/>
       <c r="C300" s="6"/>
       <c r="D300" s="28"/>
       <c r="E300" s="6"/>
@@ -12113,6 +12167,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A28:D28"/>
     <mergeCell ref="A36:D36"/>
     <mergeCell ref="A297:A298"/>
     <mergeCell ref="A299:A300"/>
@@ -12124,11 +12183,6 @@
     <mergeCell ref="B266:B267"/>
     <mergeCell ref="B297:B298"/>
     <mergeCell ref="B299:B300"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A28:D28"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="C3:C8 C10:C15 C42:C1047 C23:C27 C29:C35 C17:C21" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>